<commit_message>
- Added new metrics for ignoring extra attributes from actual cells - Added all the configuration for LLM Bench for Spider 1
</commit_message>
<xml_diff>
--- a/core/src/test/resources/llm-bench/spider1/queries.xlsx
+++ b/core/src/test/resources/llm-bench/spider1/queries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzoveltri/git/galois/core/src/test/resources/llm-bench/spider1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37860E1-E3CF-E540-86E1-2EDF6C30BA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE14F160-D66A-7340-A0C8-228E45E623AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="254">
   <si>
     <t>db_id</t>
   </si>
@@ -754,9 +754,6 @@
     <t>SELECT lowest_elevation_in_meters FROM usa_highlow WHERE lowest_point  =  'death valley';</t>
   </si>
   <si>
-    <t>SELECT t1.capital FROM usa_highlow AS t2 JOIN state AS t1 ON t1.state_name  =  t2.state_name WHERE t2.lowest_elevation_in_meters  =  ( SELECT MIN ( lowest_elevation_in_meters ) FROM usa_highlow ) ;</t>
-  </si>
-  <si>
     <t>SELECT river_name FROM usa_river WHERE length_in_km  =  ( SELECT MAX ( length_in_km ) FROM usa_river WHERE traverse  =  'texas' ) AND traverse  =  'texas';</t>
   </si>
   <si>
@@ -766,18 +763,12 @@
     <t>SELECT state_name FROM usa_highlow WHERE highest_elevation_in_meters  =  ( SELECT MAX ( highest_elevation_in_meters ) FROM usa_highlow );</t>
   </si>
   <si>
-    <t>SELECT t1.capital FROM usa_highlow AS t2 JOIN state AS t1 ON t1.state_name  =  t2.state_name WHERE t2.highest_elevation_in_meters  =  ( SELECT MAX ( highest_elevation_in_meters ) FROM usa_highlow );</t>
-  </si>
-  <si>
     <t>SELECT mountain_name FROM usa_mountain WHERE mountain_altitude_in_meters  =  ( SELECT MAX ( mountain_altitude_in_meters ) FROM usa_mountain );</t>
   </si>
   <si>
     <t>SELECT mountain_altitude_in_meters FROM usa_mountain WHERE mountain_name  =  'mckinley';</t>
   </si>
   <si>
-    <t>SELECT t2.highest_point FROM usa_highlow AS t2 JOIN state AS t1 ON t1.state_name  =  t2.state_name WHERE t1.area_squared_miles  =  ( SELECT MIN ( area_squared_miles ) FROM usa_state );</t>
-  </si>
-  <si>
     <t>SELECT DISTINCT length_in_km FROM usa_river WHERE length_in_km  =  ( SELECT MAX ( length_in_km ) FROM usa_river );</t>
   </si>
   <si>
@@ -791,6 +782,27 @@
   </si>
   <si>
     <t>SELECT t2.capital FROM usa_state AS t2 JOIN usa_border_info AS t1 ON t2.state_name  =  t1.border WHERE t1.state_name  =  'texas';</t>
+  </si>
+  <si>
+    <t>SELECT t1.capital FROM usa_highlow AS t2 JOIN usa_state AS t1 ON t1.state_name  =  t2.state_name WHERE t2.lowest_elevation_in_meters  =  ( SELECT MIN ( lowest_elevation_in_meters ) FROM usa_highlow ) ;</t>
+  </si>
+  <si>
+    <t>SELECT t1.capital FROM usa_highlow AS t2 JOIN usa_state AS t1 ON t1.state_name  =  t2.state_name WHERE t2.highest_elevation_in_meters  =  ( SELECT MAX ( highest_elevation_in_meters ) FROM usa_highlow );</t>
+  </si>
+  <si>
+    <t>SELECT t2.highest_point FROM usa_highlow AS t2 JOIN usa_state AS t1 ON t1.state_name  =  t2.state_name WHERE t1.area_squared_miles  =  ( SELECT MIN ( area_squared_miles ) FROM usa_state );</t>
+  </si>
+  <si>
+    <t>SELECT t1.name FROM "cast" AS t2 JOIN actor AS t1 ON t2.aid  =  t1.aid JOIN movie AS t3 ON t3.mid  =  t2.msid WHERE t2.role  =  'Alan Turing' AND t3.title  =  'The Imitation Game';</t>
+  </si>
+  <si>
+    <t>SELECT t1.name FROM "cast" AS t3 JOIN actor AS t1 ON t3.aid  =  t1.aid JOIN tv_series AS t2 ON t2.sid  =  t3.msid WHERE t3.role  =  'Olivia Pope' AND t2.title  =  'Scandal';</t>
+  </si>
+  <si>
+    <t>SELECT t1.name FROM "cast" AS t2 JOIN actor AS t1 ON t2.aid  =  t1.aid WHERE t2.role  =  'Mr. Bean';</t>
+  </si>
+  <si>
+    <t>SELECT director FROM movie WHERE title  = 'Avatar'</t>
   </si>
 </sst>
 </file>
@@ -1084,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B157" sqref="B157"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1112,7 +1124,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -1123,7 +1135,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>253</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -1343,7 +1355,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>32</v>
@@ -1354,7 +1366,7 @@
         <v>10</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>33</v>
@@ -1365,7 +1377,7 @@
         <v>10</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>34</v>
@@ -1376,7 +1388,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>35</v>
@@ -1387,7 +1399,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>36</v>
@@ -1398,7 +1410,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>37</v>
@@ -1409,7 +1421,7 @@
         <v>10</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>38</v>
@@ -1420,7 +1432,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>39</v>
@@ -1574,7 +1586,7 @@
         <v>10</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>54</v>
@@ -1585,7 +1597,7 @@
         <v>10</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>55</v>
@@ -1596,7 +1608,7 @@
         <v>10</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>56</v>
@@ -1607,7 +1619,7 @@
         <v>10</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>57</v>
@@ -1618,7 +1630,7 @@
         <v>10</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>58</v>
@@ -1629,7 +1641,7 @@
         <v>10</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>59</v>
@@ -1640,7 +1652,7 @@
         <v>10</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>60</v>
@@ -1651,7 +1663,7 @@
         <v>10</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>61</v>
@@ -1783,7 +1795,7 @@
         <v>10</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>75</v>
@@ -1794,7 +1806,7 @@
         <v>10</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>76</v>
@@ -1805,7 +1817,7 @@
         <v>10</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>77</v>
@@ -1816,7 +1828,7 @@
         <v>10</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>78</v>
@@ -1959,7 +1971,7 @@
         <v>10</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>92</v>
@@ -1970,7 +1982,7 @@
         <v>10</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>93</v>
@@ -1981,7 +1993,7 @@
         <v>10</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>94</v>
@@ -1992,7 +2004,7 @@
         <v>10</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>95</v>
@@ -2039,7 +2051,7 @@
         <v>227</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2058,7 +2070,7 @@
         <v>10</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>104</v>
@@ -2069,7 +2081,7 @@
         <v>10</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>105</v>
@@ -2080,7 +2092,7 @@
         <v>10</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>106</v>
@@ -2091,7 +2103,7 @@
         <v>10</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>107</v>
@@ -2102,7 +2114,7 @@
         <v>10</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C92" s="2" t="s">
         <v>108</v>
@@ -2113,7 +2125,7 @@
         <v>10</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C93" s="2" t="s">
         <v>109</v>
@@ -2245,7 +2257,7 @@
         <v>10</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C105" s="2" t="s">
         <v>123</v>
@@ -2256,7 +2268,7 @@
         <v>10</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C106" s="2" t="s">
         <v>124</v>
@@ -2267,7 +2279,7 @@
         <v>10</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C107" s="2" t="s">
         <v>125</v>
@@ -2278,7 +2290,7 @@
         <v>10</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>126</v>
@@ -2289,7 +2301,7 @@
         <v>10</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>127</v>
@@ -2300,7 +2312,7 @@
         <v>10</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>128</v>
@@ -2311,7 +2323,7 @@
         <v>10</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>129</v>
@@ -2322,7 +2334,7 @@
         <v>10</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>130</v>
@@ -2399,7 +2411,7 @@
         <v>10</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>139</v>
@@ -2476,7 +2488,7 @@
         <v>10</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>149</v>
@@ -2487,7 +2499,7 @@
         <v>10</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>151</v>
@@ -2498,7 +2510,7 @@
         <v>10</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>152</v>
@@ -2509,7 +2521,7 @@
         <v>10</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>244</v>
+        <v>249</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>154</v>
@@ -2652,7 +2664,7 @@
         <v>157</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
       <c r="C142" s="2" t="s">
         <v>169</v>
@@ -2663,7 +2675,7 @@
         <v>157</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
       <c r="C143" s="2" t="s">
         <v>170</v>
@@ -2674,7 +2686,7 @@
         <v>157</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
       <c r="C144" s="2" t="s">
         <v>171</v>
@@ -2685,7 +2697,7 @@
         <v>157</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
       <c r="C145" s="2" t="s">
         <v>172</v>
@@ -2696,7 +2708,7 @@
         <v>157</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>173</v>
@@ -2718,7 +2730,7 @@
         <v>157</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>207</v>
+        <v>251</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>175</v>
@@ -2751,7 +2763,7 @@
         <v>157</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>209</v>
+        <v>252</v>
       </c>
       <c r="C151" s="2" t="s">
         <v>178</v>

</xml_diff>